<commit_message>
Conversion error (off by 1000) correction in land/BLAPE
</commit_message>
<xml_diff>
--- a/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
+++ b/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_EI+Agora/land/BLAPE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\land\BLAPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{935415E4-AC1B-44C6-B245-0542F1965718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7268252-48F9-450E-9716-2F17F11CD07D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248BD58-E56D-4F11-8131-16BF24787BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -574,22 +574,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" customWidth="1"/>
-    <col min="2" max="2" width="51.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -597,61 +597,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="3"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="9"/>
     </row>
   </sheetData>
@@ -667,19 +667,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -687,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -695,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -703,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -711,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -719,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -727,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -735,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -743,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -751,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -759,7 +761,7 @@
         <v>4.2997168577917945E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -767,7 +769,7 @@
         <v>3.5003753313133949E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -788,16 +790,16 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.54296875" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" customWidth="1"/>
-    <col min="3" max="29" width="8.7265625" customWidth="1"/>
-    <col min="30" max="30" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="31" max="47" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="62.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="29" width="8.7109375" customWidth="1"/>
+    <col min="30" max="30" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="47" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -940,7 +942,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1041,12 +1043,12 @@
         <v>-230</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1093,11 +1095,11 @@
         <v>-230.8</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1131,7 +1133,7 @@
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
     </row>
-    <row r="17" spans="2:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:47" x14ac:dyDescent="0.25">
       <c r="AH17" s="4"/>
       <c r="AI17" s="4"/>
       <c r="AJ17" s="4"/>
@@ -1147,7 +1149,7 @@
       <c r="AT17" s="4"/>
       <c r="AU17" s="4"/>
     </row>
-    <row r="21" spans="2:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
     </row>
   </sheetData>
@@ -1164,18 +1166,18 @@
   </sheetPr>
   <dimension ref="A1:AK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="17" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1273,136 +1275,136 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2">
-        <f>EEA!AF2*1000000000</f>
-        <v>-241000000000</v>
+        <f>EEA!AF2*1000000000000</f>
+        <v>-241000000000000</v>
       </c>
       <c r="C2" s="2">
         <f>EEA!AG2*1000000000</f>
         <v>-230000000000</v>
       </c>
       <c r="D2" s="2">
-        <f>EEA!AH4*1000000000</f>
-        <v>-244500000000</v>
+        <f>EEA!AH4*1000000000000</f>
+        <v>-244500000000000</v>
       </c>
       <c r="E2" s="2">
-        <f>EEA!AI4*1000000000</f>
-        <v>-239800000000</v>
+        <f>EEA!AI4*1000000000000</f>
+        <v>-239800000000000</v>
       </c>
       <c r="F2" s="2">
-        <f>EEA!AJ4*1000000000</f>
-        <v>-239700000000</v>
+        <f>EEA!AJ4*1000000000000</f>
+        <v>-239700000000000</v>
       </c>
       <c r="G2" s="2">
-        <f>EEA!AK4*1000000000</f>
-        <v>-240700000000</v>
+        <f>EEA!AK4*1000000000000</f>
+        <v>-240700000000000</v>
       </c>
       <c r="H2" s="2">
-        <f>EEA!AL4*1000000000</f>
-        <v>-237400000000</v>
+        <f>EEA!AL4*1000000000000</f>
+        <v>-237400000000000</v>
       </c>
       <c r="I2" s="2">
-        <f>EEA!AM4*1000000000</f>
-        <v>-237300000000</v>
+        <f>EEA!AM4*1000000000000</f>
+        <v>-237300000000000</v>
       </c>
       <c r="J2" s="2">
-        <f>EEA!AN4*1000000000</f>
-        <v>-236900000000</v>
+        <f>EEA!AN4*1000000000000</f>
+        <v>-236900000000000</v>
       </c>
       <c r="K2" s="2">
-        <f>EEA!AO4*1000000000</f>
-        <v>-237900000000</v>
+        <f>EEA!AO4*1000000000000</f>
+        <v>-237900000000000</v>
       </c>
       <c r="L2" s="2">
-        <f>EEA!AP4*1000000000</f>
-        <v>-239800000000</v>
+        <f>EEA!AP4*1000000000000</f>
+        <v>-239800000000000</v>
       </c>
       <c r="M2" s="2">
-        <f>EEA!AQ4*1000000000</f>
-        <v>-237700000000</v>
+        <f>EEA!AQ4*1000000000000</f>
+        <v>-237700000000000</v>
       </c>
       <c r="N2" s="2">
-        <f>EEA!AR4*1000000000</f>
-        <v>-237600000000</v>
+        <f>EEA!AR4*1000000000000</f>
+        <v>-237600000000000</v>
       </c>
       <c r="O2" s="2">
-        <f>EEA!AS4*1000000000</f>
-        <v>-233300000000</v>
+        <f>EEA!AS4*1000000000000</f>
+        <v>-233300000000000</v>
       </c>
       <c r="P2" s="2">
-        <f>EEA!AT4*1000000000</f>
-        <v>-231800000000</v>
+        <f>EEA!AT4*1000000000000</f>
+        <v>-231800000000000</v>
       </c>
       <c r="Q2" s="2">
-        <f>EEA!AU4*1000000000</f>
-        <v>-230800000000</v>
+        <f>EEA!AU4*1000000000000</f>
+        <v>-230800000000000</v>
       </c>
       <c r="R2" s="7">
         <f>$Q$2+(R1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-229000000000</v>
+        <v>-229000000000000</v>
       </c>
       <c r="S2" s="7">
         <f t="shared" ref="S2:V2" si="0">$Q$2+(S1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-227200000000</v>
+        <v>-227200000000000</v>
       </c>
       <c r="T2" s="7">
         <f t="shared" si="0"/>
-        <v>-225400000000</v>
+        <v>-225400000000000</v>
       </c>
       <c r="U2" s="7">
         <f t="shared" si="0"/>
-        <v>-223600000000</v>
+        <v>-223600000000000</v>
       </c>
       <c r="V2" s="7">
         <f t="shared" si="0"/>
-        <v>-221800000000</v>
+        <v>-221800000000000</v>
       </c>
       <c r="W2" s="7">
         <f t="shared" ref="W2" si="1">$Q$2+(W1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-220000000000</v>
+        <v>-220000000000000</v>
       </c>
       <c r="X2" s="7">
         <f t="shared" ref="X2" si="2">$Q$2+(X1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-218200000000</v>
+        <v>-218200000000000</v>
       </c>
       <c r="Y2" s="7">
         <f t="shared" ref="Y2:Z2" si="3">$Q$2+(Y1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-216400000000</v>
+        <v>-216400000000000</v>
       </c>
       <c r="Z2" s="7">
         <f t="shared" si="3"/>
-        <v>-214600000000</v>
+        <v>-214600000000000</v>
       </c>
       <c r="AA2" s="7">
         <f t="shared" ref="AA2" si="4">$Q$2+(AA1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-212800000000</v>
+        <v>-212800000000000</v>
       </c>
       <c r="AB2" s="7">
         <f t="shared" ref="AB2" si="5">$Q$2+(AB1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-211000000000</v>
+        <v>-211000000000000</v>
       </c>
       <c r="AC2" s="7">
         <f t="shared" ref="AC2:AD2" si="6">$Q$2+(AC1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-209200000000</v>
+        <v>-209200000000000</v>
       </c>
       <c r="AD2" s="7">
         <f t="shared" si="6"/>
-        <v>-207400000000</v>
+        <v>-207400000000000</v>
       </c>
       <c r="AE2" s="7">
         <f t="shared" ref="AE2" si="7">$Q$2+(AE1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-205600000000</v>
+        <v>-205600000000000</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2" si="8">$Q$2+(AF1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-203800000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+        <v>-203800000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1598,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1696,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1794,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1892,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1990,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2186,13 +2188,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="2">
         <f>B$2*-'data from RPEpUACE'!$B11</f>
-        <v>103623176.27278225</v>
+        <v>103623176272.78224</v>
       </c>
       <c r="C11" s="2">
         <f>C$2*-'data from RPEpUACE'!$B11</f>
@@ -2200,128 +2202,128 @@
       </c>
       <c r="D11" s="2">
         <f>D$2*-'data from RPEpUACE'!$B11</f>
-        <v>105128077.17300938</v>
+        <v>105128077173.00937</v>
       </c>
       <c r="E11" s="2">
         <f>E$2*-'data from RPEpUACE'!$B11</f>
-        <v>103107210.24984723</v>
+        <v>103107210249.84723</v>
       </c>
       <c r="F11" s="2">
         <f>F$2*-'data from RPEpUACE'!$B11</f>
-        <v>103064213.08126931</v>
+        <v>103064213081.26932</v>
       </c>
       <c r="G11" s="2">
         <f>G$2*-'data from RPEpUACE'!$B11</f>
-        <v>103494184.76704849</v>
+        <v>103494184767.04849</v>
       </c>
       <c r="H11" s="2">
         <f>H$2*-'data from RPEpUACE'!$B11</f>
-        <v>102075278.2039772</v>
+        <v>102075278203.9772</v>
       </c>
       <c r="I11" s="2">
         <f>I$2*-'data from RPEpUACE'!$B11</f>
-        <v>102032281.03539929</v>
+        <v>102032281035.39928</v>
       </c>
       <c r="J11" s="2">
         <f>J$2*-'data from RPEpUACE'!$B11</f>
-        <v>101860292.36108761</v>
+        <v>101860292361.08762</v>
       </c>
       <c r="K11" s="2">
         <f>K$2*-'data from RPEpUACE'!$B11</f>
-        <v>102290264.04686679</v>
+        <v>102290264046.86679</v>
       </c>
       <c r="L11" s="2">
         <f>L$2*-'data from RPEpUACE'!$B11</f>
-        <v>103107210.24984723</v>
+        <v>103107210249.84723</v>
       </c>
       <c r="M11" s="2">
         <f>M$2*-'data from RPEpUACE'!$B11</f>
-        <v>102204269.70971096</v>
+        <v>102204269709.71095</v>
       </c>
       <c r="N11" s="2">
         <f>N$2*-'data from RPEpUACE'!$B11</f>
-        <v>102161272.54113303</v>
+        <v>102161272541.13304</v>
       </c>
       <c r="O11" s="2">
         <f>O$2*-'data from RPEpUACE'!$B11</f>
-        <v>100312394.29228257</v>
+        <v>100312394292.28256</v>
       </c>
       <c r="P11" s="2">
         <f>P$2*-'data from RPEpUACE'!$B11</f>
-        <v>99667436.76361379</v>
+        <v>99667436763.6138</v>
       </c>
       <c r="Q11" s="2">
         <f>Q$2*-'data from RPEpUACE'!$B11</f>
-        <v>99237465.077834621</v>
+        <v>99237465077.83461</v>
       </c>
       <c r="R11" s="2">
         <f>R$2*-'data from RPEpUACE'!$B11</f>
-        <v>98463516.043432087</v>
+        <v>98463516043.432098</v>
       </c>
       <c r="S11" s="2">
         <f>S$2*-'data from RPEpUACE'!$B11</f>
-        <v>97689567.009029567</v>
+        <v>97689567009.029572</v>
       </c>
       <c r="T11" s="2">
         <f>T$2*-'data from RPEpUACE'!$B11</f>
-        <v>96915617.974627048</v>
+        <v>96915617974.627045</v>
       </c>
       <c r="U11" s="2">
         <f>U$2*-'data from RPEpUACE'!$B11</f>
-        <v>96141668.940224528</v>
+        <v>96141668940.224518</v>
       </c>
       <c r="V11" s="2">
         <f>V$2*-'data from RPEpUACE'!$B11</f>
-        <v>95367719.905822009</v>
+        <v>95367719905.822006</v>
       </c>
       <c r="W11" s="2">
         <f>W$2*-'data from RPEpUACE'!$B11</f>
-        <v>94593770.871419474</v>
+        <v>94593770871.419479</v>
       </c>
       <c r="X11" s="2">
         <f>X$2*-'data from RPEpUACE'!$B11</f>
-        <v>93819821.837016955</v>
+        <v>93819821837.016953</v>
       </c>
       <c r="Y11" s="2">
         <f>Y$2*-'data from RPEpUACE'!$B11</f>
-        <v>93045872.802614436</v>
+        <v>93045872802.614426</v>
       </c>
       <c r="Z11" s="2">
         <f>Z$2*-'data from RPEpUACE'!$B11</f>
-        <v>92271923.768211916</v>
+        <v>92271923768.211914</v>
       </c>
       <c r="AA11" s="2">
         <f>AA$2*-'data from RPEpUACE'!$B11</f>
-        <v>91497974.733809382</v>
+        <v>91497974733.809387</v>
       </c>
       <c r="AB11" s="2">
         <f>AB$2*-'data from RPEpUACE'!$B11</f>
-        <v>90724025.699406862</v>
+        <v>90724025699.40686</v>
       </c>
       <c r="AC11" s="2">
         <f>AC$2*-'data from RPEpUACE'!$B11</f>
-        <v>89950076.665004343</v>
+        <v>89950076665.004333</v>
       </c>
       <c r="AD11" s="2">
         <f>AD$2*-'data from RPEpUACE'!$B11</f>
-        <v>89176127.630601823</v>
+        <v>89176127630.601822</v>
       </c>
       <c r="AE11" s="2">
         <f>AE$2*-'data from RPEpUACE'!$B11</f>
-        <v>88402178.596199289</v>
+        <v>88402178596.199295</v>
       </c>
       <c r="AF11" s="2">
         <f>AF$2*-'data from RPEpUACE'!$B11</f>
-        <v>87628229.561796769</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+        <v>87628229561.796768</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="2">
         <f>B$2*-'data from RPEpUACE'!$B12</f>
-        <v>8435904.5484652817</v>
+        <v>8435904548.4652815</v>
       </c>
       <c r="C12" s="2">
         <f>C$2*-'data from RPEpUACE'!$B12</f>
@@ -2329,122 +2331,122 @@
       </c>
       <c r="D12" s="2">
         <f>D$2*-'data from RPEpUACE'!$B12</f>
-        <v>8558417.6850612499</v>
+        <v>8558417685.0612507</v>
       </c>
       <c r="E12" s="2">
         <f>E$2*-'data from RPEpUACE'!$B12</f>
-        <v>8393900.0444895215</v>
+        <v>8393900044.489521</v>
       </c>
       <c r="F12" s="2">
         <f>F$2*-'data from RPEpUACE'!$B12</f>
-        <v>8390399.6691582073</v>
+        <v>8390399669.1582079</v>
       </c>
       <c r="G12" s="2">
         <f>G$2*-'data from RPEpUACE'!$B12</f>
-        <v>8425403.4224713407</v>
+        <v>8425403422.4713411</v>
       </c>
       <c r="H12" s="2">
         <f>H$2*-'data from RPEpUACE'!$B12</f>
-        <v>8309891.0365379993</v>
+        <v>8309891036.5379992</v>
       </c>
       <c r="I12" s="2">
         <f>I$2*-'data from RPEpUACE'!$B12</f>
-        <v>8306390.6612066859</v>
+        <v>8306390661.206686</v>
       </c>
       <c r="J12" s="2">
         <f>J$2*-'data from RPEpUACE'!$B12</f>
-        <v>8292389.1598814325</v>
+        <v>8292389159.8814325</v>
       </c>
       <c r="K12" s="2">
         <f>K$2*-'data from RPEpUACE'!$B12</f>
-        <v>8327392.913194566</v>
+        <v>8327392913.1945667</v>
       </c>
       <c r="L12" s="2">
         <f>L$2*-'data from RPEpUACE'!$B12</f>
-        <v>8393900.0444895215</v>
+        <v>8393900044.489521</v>
       </c>
       <c r="M12" s="2">
         <f>M$2*-'data from RPEpUACE'!$B12</f>
-        <v>8320392.1625319393</v>
+        <v>8320392162.5319395</v>
       </c>
       <c r="N12" s="2">
         <f>N$2*-'data from RPEpUACE'!$B12</f>
-        <v>8316891.787200626</v>
+        <v>8316891787.2006264</v>
       </c>
       <c r="O12" s="2">
         <f>O$2*-'data from RPEpUACE'!$B12</f>
-        <v>8166375.6479541501</v>
+        <v>8166375647.9541502</v>
       </c>
       <c r="P12" s="2">
         <f>P$2*-'data from RPEpUACE'!$B12</f>
-        <v>8113870.0179844489</v>
+        <v>8113870017.9844494</v>
       </c>
       <c r="Q12" s="2">
         <f>Q$2*-'data from RPEpUACE'!$B12</f>
-        <v>8078866.2646713154</v>
+        <v>8078866264.6713152</v>
       </c>
       <c r="R12" s="2">
         <f>R$2*-'data from RPEpUACE'!$B12</f>
-        <v>8015859.5087076742</v>
+        <v>8015859508.707674</v>
       </c>
       <c r="S12" s="2">
         <f>S$2*-'data from RPEpUACE'!$B12</f>
-        <v>7952852.752744033</v>
+        <v>7952852752.7440329</v>
       </c>
       <c r="T12" s="2">
         <f>T$2*-'data from RPEpUACE'!$B12</f>
-        <v>7889845.9967803918</v>
+        <v>7889845996.7803917</v>
       </c>
       <c r="U12" s="2">
         <f>U$2*-'data from RPEpUACE'!$B12</f>
-        <v>7826839.2408167506</v>
+        <v>7826839240.8167505</v>
       </c>
       <c r="V12" s="2">
         <f>V$2*-'data from RPEpUACE'!$B12</f>
-        <v>7763832.4848531093</v>
+        <v>7763832484.8531094</v>
       </c>
       <c r="W12" s="2">
         <f>W$2*-'data from RPEpUACE'!$B12</f>
-        <v>7700825.7288894691</v>
+        <v>7700825728.8894691</v>
       </c>
       <c r="X12" s="2">
         <f>X$2*-'data from RPEpUACE'!$B12</f>
-        <v>7637818.9729258278</v>
+        <v>7637818972.925828</v>
       </c>
       <c r="Y12" s="2">
         <f>Y$2*-'data from RPEpUACE'!$B12</f>
-        <v>7574812.2169621866</v>
+        <v>7574812216.9621868</v>
       </c>
       <c r="Z12" s="2">
         <f>Z$2*-'data from RPEpUACE'!$B12</f>
-        <v>7511805.4609985454</v>
+        <v>7511805460.9985456</v>
       </c>
       <c r="AA12" s="2">
         <f>AA$2*-'data from RPEpUACE'!$B12</f>
-        <v>7448798.7050349042</v>
+        <v>7448798705.0349045</v>
       </c>
       <c r="AB12" s="2">
         <f>AB$2*-'data from RPEpUACE'!$B12</f>
-        <v>7385791.949071263</v>
+        <v>7385791949.0712633</v>
       </c>
       <c r="AC12" s="2">
         <f>AC$2*-'data from RPEpUACE'!$B12</f>
-        <v>7322785.1931076217</v>
+        <v>7322785193.1076221</v>
       </c>
       <c r="AD12" s="2">
         <f>AD$2*-'data from RPEpUACE'!$B12</f>
-        <v>7259778.4371439805</v>
+        <v>7259778437.143981</v>
       </c>
       <c r="AE12" s="2">
         <f>AE$2*-'data from RPEpUACE'!$B12</f>
-        <v>7196771.6811803402</v>
+        <v>7196771681.1803398</v>
       </c>
       <c r="AF12" s="2">
         <f>AF$2*-'data from RPEpUACE'!$B12</f>
-        <v>7133764.925216699</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+        <v>7133764925.2166986</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2542,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -2565,26 +2567,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -2807,10 +2789,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B315-99D3-40D6-8CDB-A2BD32864BD9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCCDFE39-51E1-4773-AF71-6EA6E8E362CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2827,5 +2840,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCCDFE39-51E1-4773-AF71-6EA6E8E362CB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B315-99D3-40D6-8CDB-A2BD32864BD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Calibrates land use to 2023 projections
</commit_message>
<xml_diff>
--- a/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
+++ b/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\land\BLAPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\land\BLAPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248BD58-E56D-4F11-8131-16BF24787BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2712B04F-5F48-4950-BBE5-F7CB24659BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14820" windowHeight="9880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>BLAPE BAU LULUCF Anthropogenic Pollutant Emissions</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>g pollutant</t>
+  </si>
+  <si>
+    <t>https://www.eea.europa.eu/en/analysis/publications/trends-and-projections-in-europe-2024</t>
+  </si>
+  <si>
+    <t>calibrated to 2022 reported levels and 2023 estimated levels</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +235,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -243,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -267,6 +279,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -574,22 +590,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="51.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -597,61 +613,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="12">
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I17" s="3"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I19" s="9"/>
     </row>
   </sheetData>
@@ -671,17 +687,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -689,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -697,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -705,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -713,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -721,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -729,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -737,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -745,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -753,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -761,7 +777,7 @@
         <v>4.2997168577917945E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -769,7 +785,7 @@
         <v>3.5003753313133949E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -786,20 +802,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="62.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
-    <col min="3" max="29" width="8.7109375" customWidth="1"/>
-    <col min="30" max="30" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="47" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="62.54296875" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" customWidth="1"/>
+    <col min="3" max="29" width="8.7265625" customWidth="1"/>
+    <col min="30" max="30" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="47" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -942,7 +958,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1043,12 +1059,12 @@
         <v>-230</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1095,11 +1111,29 @@
         <v>-230.8</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AH5" s="13">
+        <v>-241</v>
+      </c>
+      <c r="AI5" s="13">
+        <v>-262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="B16" s="11"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1133,7 +1167,7 @@
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
     </row>
-    <row r="17" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:47" x14ac:dyDescent="0.35">
       <c r="AH17" s="4"/>
       <c r="AI17" s="4"/>
       <c r="AJ17" s="4"/>
@@ -1149,7 +1183,7 @@
       <c r="AT17" s="4"/>
       <c r="AU17" s="4"/>
     </row>
-    <row r="21" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B21" s="8"/>
     </row>
   </sheetData>
@@ -1167,17 +1201,17 @@
   <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:Q2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="17" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1275,7 +1309,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1288,123 +1322,123 @@
         <v>-230000000000</v>
       </c>
       <c r="D2" s="2">
-        <f>EEA!AH4*1000000000000</f>
-        <v>-244500000000000</v>
+        <f>EEA!AH5*1000000000000</f>
+        <v>-241000000000000</v>
       </c>
       <c r="E2" s="2">
-        <f>EEA!AI4*1000000000000</f>
-        <v>-239800000000000</v>
+        <f>EEA!AI5*1000000000000</f>
+        <v>-262000000000000</v>
       </c>
       <c r="F2" s="2">
-        <f>EEA!AJ4*1000000000000</f>
-        <v>-239700000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AI4*1000000000000</f>
+        <v>-261890742285237.66</v>
       </c>
       <c r="G2" s="2">
-        <f>EEA!AK4*1000000000000</f>
-        <v>-240700000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AJ4*1000000000000</f>
+        <v>-262000000000000</v>
       </c>
       <c r="H2" s="2">
-        <f>EEA!AL4*1000000000000</f>
-        <v>-237400000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AK4*1000000000000</f>
+        <v>-260911508101371</v>
       </c>
       <c r="I2" s="2">
-        <f>EEA!AM4*1000000000000</f>
-        <v>-237300000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AL4*1000000000000</f>
+        <v>-264538331929233.31</v>
       </c>
       <c r="J2" s="2">
-        <f>EEA!AN4*1000000000000</f>
-        <v>-236900000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AM4*1000000000000</f>
+        <v>-264649810366624.47</v>
       </c>
       <c r="K2" s="2">
-        <f>EEA!AO4*1000000000000</f>
-        <v>-237900000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AN4*1000000000000</f>
+        <v>-265096665259603.19</v>
       </c>
       <c r="L2" s="2">
-        <f>EEA!AP4*1000000000000</f>
-        <v>-239800000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AO4*1000000000000</f>
+        <v>-263982345523329.13</v>
       </c>
       <c r="M2" s="2">
-        <f>EEA!AQ4*1000000000000</f>
-        <v>-237700000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AP4*1000000000000</f>
+        <v>-261890742285237.66</v>
       </c>
       <c r="N2" s="2">
-        <f>EEA!AR4*1000000000000</f>
-        <v>-237600000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AQ4*1000000000000</f>
+        <v>-264204459402608.34</v>
       </c>
       <c r="O2" s="2">
-        <f>EEA!AS4*1000000000000</f>
-        <v>-233300000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AR4*1000000000000</f>
+        <v>-264315656565656.53</v>
       </c>
       <c r="P2" s="2">
-        <f>EEA!AT4*1000000000000</f>
-        <v>-231800000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AS4*1000000000000</f>
+        <v>-269187312473210.41</v>
       </c>
       <c r="Q2" s="2">
-        <f>EEA!AU4*1000000000000</f>
-        <v>-230800000000000</v>
+        <f>EEA!$AI5*EEA!$AJ4/EEA!AT4*1000000000000</f>
+        <v>-270929249352890.41</v>
       </c>
       <c r="R2" s="7">
-        <f>$Q$2+(R1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-229000000000000</v>
+        <f>Q2</f>
+        <v>-270929249352890.41</v>
       </c>
       <c r="S2" s="7">
-        <f t="shared" ref="S2:V2" si="0">$Q$2+(S1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-227200000000000</v>
+        <f t="shared" ref="S2:AF2" si="0">R2</f>
+        <v>-270929249352890.41</v>
       </c>
       <c r="T2" s="7">
         <f t="shared" si="0"/>
-        <v>-225400000000000</v>
+        <v>-270929249352890.41</v>
       </c>
       <c r="U2" s="7">
         <f t="shared" si="0"/>
-        <v>-223600000000000</v>
+        <v>-270929249352890.41</v>
       </c>
       <c r="V2" s="7">
         <f t="shared" si="0"/>
-        <v>-221800000000000</v>
+        <v>-270929249352890.41</v>
       </c>
       <c r="W2" s="7">
-        <f t="shared" ref="W2" si="1">$Q$2+(W1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-220000000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="X2" s="7">
-        <f t="shared" ref="X2" si="2">$Q$2+(X1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-218200000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="Y2" s="7">
-        <f t="shared" ref="Y2:Z2" si="3">$Q$2+(Y1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-216400000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="Z2" s="7">
-        <f t="shared" si="3"/>
-        <v>-214600000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="AA2" s="7">
-        <f t="shared" ref="AA2" si="4">$Q$2+(AA1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-212800000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="AB2" s="7">
-        <f t="shared" ref="AB2" si="5">$Q$2+(AB1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-211000000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="AC2" s="7">
-        <f t="shared" ref="AC2:AD2" si="6">$Q$2+(AC1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-209200000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="AD2" s="7">
-        <f t="shared" si="6"/>
-        <v>-207400000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="AE2" s="7">
-        <f t="shared" ref="AE2" si="7">$Q$2+(AE1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-205600000000000</v>
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
       </c>
       <c r="AF2" s="7">
-        <f t="shared" ref="AF2" si="8">$Q$2+(AF1-$Q$1)*($Q$2-$L$2)/($Q$1-$L$1)</f>
-        <v>-203800000000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-270929249352890.41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1502,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1698,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1796,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1894,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1992,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2090,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2188,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2202,122 +2236,122 @@
       </c>
       <c r="D11" s="2">
         <f>D$2*-'data from RPEpUACE'!$B11</f>
-        <v>105128077173.00937</v>
+        <v>103623176272.78224</v>
       </c>
       <c r="E11" s="2">
         <f>E$2*-'data from RPEpUACE'!$B11</f>
-        <v>103107210249.84723</v>
+        <v>112652581674.14502</v>
       </c>
       <c r="F11" s="2">
         <f>F$2*-'data from RPEpUACE'!$B11</f>
-        <v>103064213081.26932</v>
+        <v>112605603950.34427</v>
       </c>
       <c r="G11" s="2">
         <f>G$2*-'data from RPEpUACE'!$B11</f>
-        <v>103494184767.04849</v>
+        <v>112652581674.14502</v>
       </c>
       <c r="H11" s="2">
         <f>H$2*-'data from RPEpUACE'!$B11</f>
-        <v>102075278203.9772</v>
+        <v>112184560977.53453</v>
       </c>
       <c r="I11" s="2">
         <f>I$2*-'data from RPEpUACE'!$B11</f>
-        <v>102032281035.39928</v>
+        <v>113743992532.82458</v>
       </c>
       <c r="J11" s="2">
         <f>J$2*-'data from RPEpUACE'!$B11</f>
-        <v>101860292361.08762</v>
+        <v>113791925104.47769</v>
       </c>
       <c r="K11" s="2">
         <f>K$2*-'data from RPEpUACE'!$B11</f>
-        <v>102290264046.86679</v>
+        <v>113984060056.11041</v>
       </c>
       <c r="L11" s="2">
         <f>L$2*-'data from RPEpUACE'!$B11</f>
-        <v>103107210249.84723</v>
+        <v>113504934120.60765</v>
       </c>
       <c r="M11" s="2">
         <f>M$2*-'data from RPEpUACE'!$B11</f>
-        <v>102204269709.71095</v>
+        <v>112605603950.34427</v>
       </c>
       <c r="N11" s="2">
         <f>N$2*-'data from RPEpUACE'!$B11</f>
-        <v>102161272541.13304</v>
+        <v>113600436799.71629</v>
       </c>
       <c r="O11" s="2">
         <f>O$2*-'data from RPEpUACE'!$B11</f>
-        <v>100312394292.28256</v>
+        <v>113648248431.36598</v>
       </c>
       <c r="P11" s="2">
         <f>P$2*-'data from RPEpUACE'!$B11</f>
-        <v>99667436763.6138</v>
+        <v>115742922534.47302</v>
       </c>
       <c r="Q11" s="2">
         <f>Q$2*-'data from RPEpUACE'!$B11</f>
-        <v>99237465077.83461</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="R11" s="2">
         <f>R$2*-'data from RPEpUACE'!$B11</f>
-        <v>98463516043.432098</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="S11" s="2">
         <f>S$2*-'data from RPEpUACE'!$B11</f>
-        <v>97689567009.029572</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="T11" s="2">
         <f>T$2*-'data from RPEpUACE'!$B11</f>
-        <v>96915617974.627045</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="U11" s="2">
         <f>U$2*-'data from RPEpUACE'!$B11</f>
-        <v>96141668940.224518</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="V11" s="2">
         <f>V$2*-'data from RPEpUACE'!$B11</f>
-        <v>95367719905.822006</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="W11" s="2">
         <f>W$2*-'data from RPEpUACE'!$B11</f>
-        <v>94593770871.419479</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="X11" s="2">
         <f>X$2*-'data from RPEpUACE'!$B11</f>
-        <v>93819821837.016953</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="Y11" s="2">
         <f>Y$2*-'data from RPEpUACE'!$B11</f>
-        <v>93045872802.614426</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="Z11" s="2">
         <f>Z$2*-'data from RPEpUACE'!$B11</f>
-        <v>92271923768.211914</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="AA11" s="2">
         <f>AA$2*-'data from RPEpUACE'!$B11</f>
-        <v>91497974733.809387</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="AB11" s="2">
         <f>AB$2*-'data from RPEpUACE'!$B11</f>
-        <v>90724025699.40686</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="AC11" s="2">
         <f>AC$2*-'data from RPEpUACE'!$B11</f>
-        <v>89950076665.004333</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="AD11" s="2">
         <f>AD$2*-'data from RPEpUACE'!$B11</f>
-        <v>89176127630.601822</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="AE11" s="2">
         <f>AE$2*-'data from RPEpUACE'!$B11</f>
-        <v>88402178596.199295</v>
+        <v>116491906071.14995</v>
       </c>
       <c r="AF11" s="2">
         <f>AF$2*-'data from RPEpUACE'!$B11</f>
-        <v>87628229561.796768</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+        <v>116491906071.14995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2331,122 +2365,122 @@
       </c>
       <c r="D12" s="2">
         <f>D$2*-'data from RPEpUACE'!$B12</f>
-        <v>8558417685.0612507</v>
+        <v>8435904548.4652815</v>
       </c>
       <c r="E12" s="2">
         <f>E$2*-'data from RPEpUACE'!$B12</f>
-        <v>8393900044.489521</v>
+        <v>9170983368.0410938</v>
       </c>
       <c r="F12" s="2">
         <f>F$2*-'data from RPEpUACE'!$B12</f>
-        <v>8390399669.1582079</v>
+        <v>9167158937.9459972</v>
       </c>
       <c r="G12" s="2">
         <f>G$2*-'data from RPEpUACE'!$B12</f>
-        <v>8425403422.4713411</v>
+        <v>9170983368.0410938</v>
       </c>
       <c r="H12" s="2">
         <f>H$2*-'data from RPEpUACE'!$B12</f>
-        <v>8309891036.5379992</v>
+        <v>9132882066.1381397</v>
       </c>
       <c r="I12" s="2">
         <f>I$2*-'data from RPEpUACE'!$B12</f>
-        <v>8306390661.206686</v>
+        <v>9259834512.7188282</v>
       </c>
       <c r="J12" s="2">
         <f>J$2*-'data from RPEpUACE'!$B12</f>
-        <v>8292389159.8814325</v>
+        <v>9263736676.4410019</v>
       </c>
       <c r="K12" s="2">
         <f>K$2*-'data from RPEpUACE'!$B12</f>
-        <v>8327392913.1945667</v>
+        <v>9279378274.8815956</v>
       </c>
       <c r="L12" s="2">
         <f>L$2*-'data from RPEpUACE'!$B12</f>
-        <v>8393900044.489521</v>
+        <v>9240372901.7211018</v>
       </c>
       <c r="M12" s="2">
         <f>M$2*-'data from RPEpUACE'!$B12</f>
-        <v>8320392162.5319395</v>
+        <v>9167158937.9459972</v>
       </c>
       <c r="N12" s="2">
         <f>N$2*-'data from RPEpUACE'!$B12</f>
-        <v>8316891787.2006264</v>
+        <v>9248147721.1588154</v>
       </c>
       <c r="O12" s="2">
         <f>O$2*-'data from RPEpUACE'!$B12</f>
-        <v>8166375647.9541502</v>
+        <v>9252040039.2232742</v>
       </c>
       <c r="P12" s="2">
         <f>P$2*-'data from RPEpUACE'!$B12</f>
-        <v>8113870017.9844494</v>
+        <v>9422566280.8377628</v>
       </c>
       <c r="Q12" s="2">
         <f>Q$2*-'data from RPEpUACE'!$B12</f>
-        <v>8078866264.6713152</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="R12" s="2">
         <f>R$2*-'data from RPEpUACE'!$B12</f>
-        <v>8015859508.707674</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="S12" s="2">
         <f>S$2*-'data from RPEpUACE'!$B12</f>
-        <v>7952852752.7440329</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="T12" s="2">
         <f>T$2*-'data from RPEpUACE'!$B12</f>
-        <v>7889845996.7803917</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="U12" s="2">
         <f>U$2*-'data from RPEpUACE'!$B12</f>
-        <v>7826839240.8167505</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="V12" s="2">
         <f>V$2*-'data from RPEpUACE'!$B12</f>
-        <v>7763832484.8531094</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="W12" s="2">
         <f>W$2*-'data from RPEpUACE'!$B12</f>
-        <v>7700825728.8894691</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="X12" s="2">
         <f>X$2*-'data from RPEpUACE'!$B12</f>
-        <v>7637818972.925828</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="Y12" s="2">
         <f>Y$2*-'data from RPEpUACE'!$B12</f>
-        <v>7574812216.9621868</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="Z12" s="2">
         <f>Z$2*-'data from RPEpUACE'!$B12</f>
-        <v>7511805460.9985456</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="AA12" s="2">
         <f>AA$2*-'data from RPEpUACE'!$B12</f>
-        <v>7448798705.0349045</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="AB12" s="2">
         <f>AB$2*-'data from RPEpUACE'!$B12</f>
-        <v>7385791949.0712633</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="AC12" s="2">
         <f>AC$2*-'data from RPEpUACE'!$B12</f>
-        <v>7322785193.1076221</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="AD12" s="2">
         <f>AD$2*-'data from RPEpUACE'!$B12</f>
-        <v>7259778437.143981</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="AE12" s="2">
         <f>AE$2*-'data from RPEpUACE'!$B12</f>
-        <v>7196771681.1803398</v>
+        <v>9483540609.6611309</v>
       </c>
       <c r="AF12" s="2">
         <f>AF$2*-'data from RPEpUACE'!$B12</f>
-        <v>7133764925.2166986</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+        <v>9483540609.6611309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2544,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -2567,6 +2601,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -2789,17 +2834,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2810,6 +2844,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEC1591-6001-4F0F-89DA-9084D560F9F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCCDFE39-51E1-4773-AF71-6EA6E8E362CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2828,17 +2873,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEC1591-6001-4F0F-89DA-9084D560F9F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B315-99D3-40D6-8CDB-A2BD32864BD9}">
   <ds:schemaRefs>

</xml_diff>